<commit_message>
Update for March 14.
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFDAC93-0C4B-1246-B717-97D11C5A49E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D4EEB5-9EE3-9847-9ED3-8992DD846BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{52E8CECD-B562-9649-AE5E-9D9A22BA9B75}"/>
   </bookViews>
   <sheets>
     <sheet name="Ontario" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Cases Since Feb 23</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/toronto-covid-19-march-14-1.5497959</t>
   </si>
 </sst>
 </file>
@@ -275,10 +278,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Ontario!$E$5:$E$19</c:f>
+              <c:f>Ontario!$E$5:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -323,16 +326,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Ontario!$C$5:$C$19</c:f>
+              <c:f>Ontario!$C$5:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -377,6 +383,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1255,15 +1264,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>425450</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1588,11 +1597,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A9237A-1352-3E4D-BF1A-5255317D7F41}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1662,15 +1669,15 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C19" si="0">B3-$B$4</f>
+        <f t="shared" ref="C3:C20" si="0">B3-$B$4</f>
         <v>-1</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D19" si="1">A3-$A$2</f>
+        <f t="shared" ref="D3:D20" si="1">A3-$A$2</f>
         <v>2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E19" si="2">A3-$A$5</f>
+        <f t="shared" ref="E3:E20" si="2">A3-$A$5</f>
         <v>-27</v>
       </c>
       <c r="F3">
@@ -2167,6 +2174,37 @@
       </c>
       <c r="H19" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43904</v>
+      </c>
+      <c r="B20">
+        <v>103</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ref="F20" si="6">E20-E19</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" ref="G20" si="7">(C20/C19)^(1/F20)-1</f>
+        <v>0.31578947368421062</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2189,8 +2227,9 @@
     <hyperlink ref="H7" r:id="rId16" xr:uid="{ADBB449F-89CB-B241-9EB7-739EEEF97803}"/>
     <hyperlink ref="H8" r:id="rId17" xr:uid="{C402538B-E213-5E4D-A98B-0C5CCD007ADC}"/>
     <hyperlink ref="H2" r:id="rId18" xr:uid="{836CF848-D4B9-FE47-9961-ED6DA8418687}"/>
+    <hyperlink ref="H20" r:id="rId19" xr:uid="{14532B07-9853-C348-857E-7B8B340A8F90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add README.md and update graphs
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D4EEB5-9EE3-9847-9ED3-8992DD846BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C83E89-5E97-5B4E-9E5B-24B27F2ED543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{52E8CECD-B562-9649-AE5E-9D9A22BA9B75}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -105,12 +105,6 @@
   </si>
   <si>
     <t>Day Gap</t>
-  </si>
-  <si>
-    <t>Days Since Feb 23</t>
-  </si>
-  <si>
-    <t>Cases Since Feb 23</t>
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/toronto-covid-19-march-14-1.5497959</t>
@@ -278,67 +272,76 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Ontario!$E$5:$E$20</c:f>
+              <c:f>Ontario!$C$2:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20</c:v>
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Ontario!$C$5:$C$20</c:f>
+              <c:f>Ontario!$B$2:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -349,43 +352,52 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>29</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>34</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>57</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>76</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>100</c:v>
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,7 +466,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Feb 23</a:t>
+                  <a:t> Jan 25</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -571,13 +583,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Cases</a:t>
+                  <a:t>Days Since Jan 25</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Since Feb 23</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1269,8 +1276,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
@@ -1597,7 +1604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A9237A-1352-3E4D-BF1A-5255317D7F41}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1605,14 +1612,12 @@
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1620,25 +1625,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43855</v>
       </c>
@@ -1646,22 +1645,14 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f>B2-$B$4</f>
-        <v>-2</v>
-      </c>
-      <c r="D2">
         <f>A2-$A$2</f>
         <v>0</v>
       </c>
-      <c r="E2">
-        <f>A2-$A$5</f>
-        <v>-29</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43857</v>
       </c>
@@ -1669,26 +1660,22 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C20" si="0">B3-$B$4</f>
-        <v>-1</v>
+        <f>A3-$A$2</f>
+        <v>2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D20" si="1">A3-$A$2</f>
+        <f>C3-C2</f>
         <v>2</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E20" si="2">A3-$A$5</f>
-        <v>-27</v>
-      </c>
-      <c r="F3">
-        <f>E3-E2</f>
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="E3" s="2">
+        <f>(B3/B2)^(1/D3)-1</f>
+        <v>0.41421356237309515</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43861</v>
       </c>
@@ -1696,26 +1683,22 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>A4-$A$2</f>
+        <v>6</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="2"/>
-        <v>-23</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F19" si="3">E4-E3</f>
+        <f t="shared" ref="D4:D20" si="0">C4-C3</f>
         <v>4</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="E4" s="2">
+        <f>(B4/B3)^(1/D4)-1</f>
+        <v>0.1066819197003217</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43884</v>
       </c>
@@ -1723,274 +1706,206 @@
         <v>4</v>
       </c>
       <c r="C5">
+        <f>A5-$A$2</f>
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E5" s="2">
+        <f>(B5/B4)^(1/D5)-1</f>
+        <v>1.2586467339374297E-2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43887</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>A6-$A$2</f>
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <f>(B6/B5)^(1/D6)-1</f>
+        <v>7.7217345015941907E-2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43888</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>A7-$A$2</f>
+        <v>33</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
+      <c r="E7" s="2">
+        <f>(B7/B6)^(1/D7)-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43889</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f>A8-$A$2</f>
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <f>(B8/B7)^(1/D8)-1</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43890</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <f>A9-$A$2</f>
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <f>(B9/B8)^(1/D9)-1</f>
+        <v>0.375</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <f>A10-$A$2</f>
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <f>(B10/B9)^(1/D10)-1</f>
+        <v>0.36363636363636354</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43892</v>
+      </c>
+      <c r="B11">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <f>A11-$A$2</f>
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <f>(B11/B10)^(1/D11)-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43893</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <f>A12-$A$2</f>
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <f>(B12/B11)^(1/D12)-1</f>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43895</v>
+      </c>
+      <c r="B13">
         <v>23</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>43887</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
+      <c r="C13">
+        <f>A13-$A$2</f>
+        <v>40</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" ref="G6:G15" si="4">(C6/C5)^(1/F6)-1</f>
-        <v>0.25992104989487319</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>20</v>
+      <c r="E13" s="2">
+        <f>(B13/B12)^(1/D13)-1</f>
+        <v>7.2380529476360866E-2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>43888</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>43889</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="4"/>
-        <v>0.66666666666666674</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>43890</v>
-      </c>
-      <c r="B9">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="4"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>43891</v>
-      </c>
-      <c r="B10">
-        <v>15</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>43892</v>
-      </c>
-      <c r="B11">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>43893</v>
-      </c>
-      <c r="B12">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="4"/>
-        <v>0.1333333333333333</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>43895</v>
-      </c>
-      <c r="B13">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="4"/>
-        <v>8.4652289093280819E-2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43896</v>
       </c>
@@ -1998,30 +1913,22 @@
         <v>28</v>
       </c>
       <c r="C14">
+        <f>A14-$A$2</f>
+        <v>41</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G14" s="2">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="E14" s="2">
+        <f>(B14/B13)^(1/D14)-1</f>
+        <v>0.21739130434782616</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
@@ -2029,30 +1936,22 @@
         <v>32</v>
       </c>
       <c r="C15">
+        <f>A15-$A$2</f>
+        <v>43</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="G15" s="2">
-        <f t="shared" si="4"/>
-        <v>7.7032961426900748E-2</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="E15" s="2">
+        <f>(B15/B14)^(1/D15)-1</f>
+        <v>6.9044967649697586E-2</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43900</v>
       </c>
@@ -2060,30 +1959,22 @@
         <v>37</v>
       </c>
       <c r="C16">
+        <f>A16-$A$2</f>
+        <v>45</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="G16" s="2">
-        <f>(C16/C15)^(1/F16)-1</f>
-        <v>8.2780584007419389E-2</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="E16" s="2">
+        <f>(B16/B15)^(1/D16)-1</f>
+        <v>7.5290658380328335E-2</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43901</v>
       </c>
@@ -2091,30 +1982,22 @@
         <v>42</v>
       </c>
       <c r="C17">
+        <f>A17-$A$2</f>
+        <v>46</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G17" s="2">
-        <f t="shared" ref="G17:G19" si="5">(C17/C16)^(1/F17)-1</f>
-        <v>0.14705882352941169</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="E17" s="2">
+        <f>(B17/B16)^(1/D17)-1</f>
+        <v>0.13513513513513509</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43902</v>
       </c>
@@ -2122,30 +2005,22 @@
         <v>60</v>
       </c>
       <c r="C18">
+        <f>A18-$A$2</f>
+        <v>47</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G18" s="2">
-        <f t="shared" si="5"/>
-        <v>0.46153846153846145</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="E18" s="2">
+        <f>(B18/B17)^(1/D18)-1</f>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43903</v>
       </c>
@@ -2153,30 +2028,22 @@
         <v>79</v>
       </c>
       <c r="C19">
+        <f>A19-$A$2</f>
+        <v>48</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G19" s="2">
-        <f t="shared" si="5"/>
-        <v>0.33333333333333326</v>
-      </c>
-      <c r="H19" s="3" t="s">
+      <c r="E19" s="2">
+        <f>(B19/B18)^(1/D19)-1</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43904</v>
       </c>
@@ -2184,50 +2051,42 @@
         <v>103</v>
       </c>
       <c r="C20">
+        <f>A20-$A$2</f>
+        <v>49</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="F20">
-        <f t="shared" ref="F20" si="6">E20-E19</f>
         <v>1</v>
       </c>
-      <c r="G20" s="2">
-        <f t="shared" ref="G20" si="7">(C20/C19)^(1/F20)-1</f>
-        <v>0.31578947368421062</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>26</v>
+      <c r="E20" s="2">
+        <f>(B20/B19)^(1/D20)-1</f>
+        <v>0.30379746835443044</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H19" r:id="rId1" xr:uid="{3BC06DD8-1C63-2A4C-8A9E-4A19047DD22C}"/>
-    <hyperlink ref="H9" r:id="rId2" xr:uid="{3C89D393-F689-FF47-8088-FFA957C54119}"/>
-    <hyperlink ref="H10" r:id="rId3" xr:uid="{EA3E43BA-BFF4-9C40-B63C-84926F27C27D}"/>
-    <hyperlink ref="H11" r:id="rId4" xr:uid="{171C8763-89F5-7E4F-88BC-7A0EA89B85D5}"/>
-    <hyperlink ref="H12" r:id="rId5" xr:uid="{82BD3B5B-C242-4E42-9ABC-C1399D16A6F1}"/>
-    <hyperlink ref="H13" r:id="rId6" xr:uid="{A7DE2133-3CE9-094B-9275-BBEBE0F66E3A}"/>
-    <hyperlink ref="H14" r:id="rId7" xr:uid="{31168212-B833-9745-90EB-D87CA8F4357E}"/>
-    <hyperlink ref="H15" r:id="rId8" xr:uid="{268C4708-7DC2-314B-9749-796D12F7E880}"/>
-    <hyperlink ref="H16" r:id="rId9" xr:uid="{29CA4407-45EB-BB41-BD80-2829DD24604B}"/>
-    <hyperlink ref="H17" r:id="rId10" xr:uid="{43B53690-B17A-A44B-81C3-40F7FD89E575}"/>
-    <hyperlink ref="H18" r:id="rId11" xr:uid="{A2B24F3C-7C75-9648-9F50-2DFF415C57E9}"/>
-    <hyperlink ref="H3" r:id="rId12" xr:uid="{A264EE7C-CB8A-F347-BAFA-CFDFCAB22BEE}"/>
-    <hyperlink ref="H4" r:id="rId13" xr:uid="{104469C6-496F-EC4F-A7AB-D10705F8150E}"/>
-    <hyperlink ref="H5" r:id="rId14" xr:uid="{A5943F82-177A-AC4C-B541-DBD1B68C3C0A}"/>
-    <hyperlink ref="H6" r:id="rId15" xr:uid="{EB150305-E1F8-9D4F-B1B4-376A9B89555A}"/>
-    <hyperlink ref="H7" r:id="rId16" xr:uid="{ADBB449F-89CB-B241-9EB7-739EEEF97803}"/>
-    <hyperlink ref="H8" r:id="rId17" xr:uid="{C402538B-E213-5E4D-A98B-0C5CCD007ADC}"/>
-    <hyperlink ref="H2" r:id="rId18" xr:uid="{836CF848-D4B9-FE47-9961-ED6DA8418687}"/>
-    <hyperlink ref="H20" r:id="rId19" xr:uid="{14532B07-9853-C348-857E-7B8B340A8F90}"/>
+    <hyperlink ref="F19" r:id="rId1" xr:uid="{3BC06DD8-1C63-2A4C-8A9E-4A19047DD22C}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{3C89D393-F689-FF47-8088-FFA957C54119}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{EA3E43BA-BFF4-9C40-B63C-84926F27C27D}"/>
+    <hyperlink ref="F11" r:id="rId4" xr:uid="{171C8763-89F5-7E4F-88BC-7A0EA89B85D5}"/>
+    <hyperlink ref="F12" r:id="rId5" xr:uid="{82BD3B5B-C242-4E42-9ABC-C1399D16A6F1}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{A7DE2133-3CE9-094B-9275-BBEBE0F66E3A}"/>
+    <hyperlink ref="F14" r:id="rId7" xr:uid="{31168212-B833-9745-90EB-D87CA8F4357E}"/>
+    <hyperlink ref="F15" r:id="rId8" xr:uid="{268C4708-7DC2-314B-9749-796D12F7E880}"/>
+    <hyperlink ref="F16" r:id="rId9" xr:uid="{29CA4407-45EB-BB41-BD80-2829DD24604B}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{43B53690-B17A-A44B-81C3-40F7FD89E575}"/>
+    <hyperlink ref="F18" r:id="rId11" xr:uid="{A2B24F3C-7C75-9648-9F50-2DFF415C57E9}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{A264EE7C-CB8A-F347-BAFA-CFDFCAB22BEE}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{104469C6-496F-EC4F-A7AB-D10705F8150E}"/>
+    <hyperlink ref="F5" r:id="rId14" xr:uid="{A5943F82-177A-AC4C-B541-DBD1B68C3C0A}"/>
+    <hyperlink ref="F6" r:id="rId15" xr:uid="{EB150305-E1F8-9D4F-B1B4-376A9B89555A}"/>
+    <hyperlink ref="F7" r:id="rId16" xr:uid="{ADBB449F-89CB-B241-9EB7-739EEEF97803}"/>
+    <hyperlink ref="F8" r:id="rId17" xr:uid="{C402538B-E213-5E4D-A98B-0C5CCD007ADC}"/>
+    <hyperlink ref="F2" r:id="rId18" xr:uid="{836CF848-D4B9-FE47-9961-ED6DA8418687}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{14532B07-9853-C348-857E-7B8B340A8F90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId20"/>

</xml_diff>

<commit_message>
Update for March 15.
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C83E89-5E97-5B4E-9E5B-24B27F2ED543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED00895E-4047-C54F-A2D9-F33A1C24F7D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{52E8CECD-B562-9649-AE5E-9D9A22BA9B75}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/toronto-covid-19-march-14-1.5497959</t>
+  </si>
+  <si>
+    <t>Tests Conducted</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/ontario-new-covid-19-cases-total-sunday-1.5498410</t>
   </si>
 </sst>
 </file>
@@ -272,10 +278,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Ontario!$C$2:$C$20</c:f>
+              <c:f>Ontario!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -332,16 +338,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Ontario!$B$2:$B$20</c:f>
+              <c:f>Ontario!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -398,6 +407,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>145</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1276,7 +1288,7 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
@@ -1604,20 +1616,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A9237A-1352-3E4D-BF1A-5255317D7F41}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1625,470 +1640,500 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43855</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <f>A2-$A$2</f>
+      <c r="D2">
+        <f t="shared" ref="D2:D21" si="0">A2-$A$2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43857</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <f>A3-$A$2</f>
+      <c r="D3">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D3">
-        <f>C3-C2</f>
+      <c r="E3">
+        <f>D3-D2</f>
         <v>2</v>
       </c>
-      <c r="E3" s="2">
-        <f>(B3/B2)^(1/D3)-1</f>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F21" si="1">(B3/B2)^(1/E3)-1</f>
         <v>0.41421356237309515</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43861</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
-        <f>A4-$A$2</f>
+      <c r="D4">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D20" si="0">C4-C3</f>
+      <c r="E4">
+        <f t="shared" ref="E4:E21" si="2">D4-D3</f>
         <v>4</v>
       </c>
-      <c r="E4" s="2">
-        <f>(B4/B3)^(1/D4)-1</f>
+      <c r="F4" s="2">
+        <f t="shared" si="1"/>
         <v>0.1066819197003217</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43884</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <f>A5-$A$2</f>
-        <v>29</v>
-      </c>
       <c r="D5">
         <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="E5" s="2">
-        <f>(B5/B4)^(1/D5)-1</f>
+      <c r="F5" s="2">
+        <f t="shared" si="1"/>
         <v>1.2586467339374297E-2</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43887</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6">
-        <f>A6-$A$2</f>
-        <v>32</v>
-      </c>
       <c r="D6">
         <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E6" s="2">
-        <f>(B6/B5)^(1/D6)-1</f>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
         <v>7.7217345015941907E-2</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43888</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7">
-        <f>A7-$A$2</f>
-        <v>33</v>
-      </c>
       <c r="D7">
         <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E7" s="2">
-        <f>(B7/B6)^(1/D7)-1</f>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43889</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
-      <c r="C8">
-        <f>A8-$A$2</f>
-        <v>34</v>
-      </c>
       <c r="D8">
         <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E8" s="2">
-        <f>(B8/B7)^(1/D8)-1</f>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43890</v>
       </c>
       <c r="B9">
         <v>11</v>
       </c>
-      <c r="C9">
-        <f>A9-$A$2</f>
-        <v>35</v>
-      </c>
       <c r="D9">
         <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E9" s="2">
-        <f>(B9/B8)^(1/D9)-1</f>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
         <v>0.375</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43891</v>
       </c>
       <c r="B10">
         <v>15</v>
       </c>
-      <c r="C10">
-        <f>A10-$A$2</f>
-        <v>36</v>
-      </c>
       <c r="D10">
         <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E10" s="2">
-        <f>(B10/B9)^(1/D10)-1</f>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
         <v>0.36363636363636354</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
       <c r="B11">
         <v>18</v>
       </c>
-      <c r="C11">
-        <f>A11-$A$2</f>
-        <v>37</v>
-      </c>
       <c r="D11">
         <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E11" s="2">
-        <f>(B11/B10)^(1/D11)-1</f>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43893</v>
       </c>
       <c r="B12">
         <v>20</v>
       </c>
-      <c r="C12">
-        <f>A12-$A$2</f>
-        <v>38</v>
-      </c>
       <c r="D12">
         <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E12" s="2">
-        <f>(B12/B11)^(1/D12)-1</f>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
         <v>0.11111111111111116</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43895</v>
       </c>
       <c r="B13">
         <v>23</v>
       </c>
-      <c r="C13">
-        <f>A13-$A$2</f>
-        <v>40</v>
-      </c>
       <c r="D13">
         <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E13" s="2">
-        <f>(B13/B12)^(1/D13)-1</f>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
         <v>7.2380529476360866E-2</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43896</v>
       </c>
       <c r="B14">
         <v>28</v>
       </c>
-      <c r="C14">
-        <f>A14-$A$2</f>
-        <v>41</v>
-      </c>
       <c r="D14">
         <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E14" s="2">
-        <f>(B14/B13)^(1/D14)-1</f>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
         <v>0.21739130434782616</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
       <c r="B15">
         <v>32</v>
       </c>
-      <c r="C15">
-        <f>A15-$A$2</f>
-        <v>43</v>
-      </c>
       <c r="D15">
         <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E15" s="2">
-        <f>(B15/B14)^(1/D15)-1</f>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
         <v>6.9044967649697586E-2</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43900</v>
       </c>
       <c r="B16">
         <v>37</v>
       </c>
-      <c r="C16">
-        <f>A16-$A$2</f>
-        <v>45</v>
-      </c>
       <c r="D16">
         <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E16" s="2">
-        <f>(B16/B15)^(1/D16)-1</f>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
         <v>7.5290658380328335E-2</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43901</v>
       </c>
       <c r="B17">
         <v>42</v>
       </c>
-      <c r="C17">
-        <f>A17-$A$2</f>
-        <v>46</v>
-      </c>
       <c r="D17">
         <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E17" s="2">
-        <f>(B17/B16)^(1/D17)-1</f>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
         <v>0.13513513513513509</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43902</v>
       </c>
       <c r="B18">
         <v>60</v>
       </c>
-      <c r="C18">
-        <f>A18-$A$2</f>
-        <v>47</v>
-      </c>
       <c r="D18">
         <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E18" s="2">
-        <f>(B18/B17)^(1/D18)-1</f>
+      <c r="F18" s="2">
+        <f t="shared" si="1"/>
         <v>0.4285714285714286</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43903</v>
       </c>
       <c r="B19">
         <v>79</v>
       </c>
-      <c r="C19">
-        <f>A19-$A$2</f>
-        <v>48</v>
-      </c>
       <c r="D19">
         <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E19" s="2">
-        <f>(B19/B18)^(1/D19)-1</f>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
         <v>0.31666666666666665</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43904</v>
       </c>
       <c r="B20">
         <v>103</v>
       </c>
-      <c r="C20">
-        <f>A20-$A$2</f>
-        <v>49</v>
-      </c>
       <c r="D20">
         <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E20" s="2">
-        <f>(B20/B19)^(1/D20)-1</f>
+      <c r="F20" s="2">
+        <f t="shared" si="1"/>
         <v>0.30379746835443044</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43905</v>
+      </c>
+      <c r="B21">
+        <v>145</v>
+      </c>
+      <c r="C21">
+        <v>8462</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40776699029126218</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F19" r:id="rId1" xr:uid="{3BC06DD8-1C63-2A4C-8A9E-4A19047DD22C}"/>
-    <hyperlink ref="F9" r:id="rId2" xr:uid="{3C89D393-F689-FF47-8088-FFA957C54119}"/>
-    <hyperlink ref="F10" r:id="rId3" xr:uid="{EA3E43BA-BFF4-9C40-B63C-84926F27C27D}"/>
-    <hyperlink ref="F11" r:id="rId4" xr:uid="{171C8763-89F5-7E4F-88BC-7A0EA89B85D5}"/>
-    <hyperlink ref="F12" r:id="rId5" xr:uid="{82BD3B5B-C242-4E42-9ABC-C1399D16A6F1}"/>
-    <hyperlink ref="F13" r:id="rId6" xr:uid="{A7DE2133-3CE9-094B-9275-BBEBE0F66E3A}"/>
-    <hyperlink ref="F14" r:id="rId7" xr:uid="{31168212-B833-9745-90EB-D87CA8F4357E}"/>
-    <hyperlink ref="F15" r:id="rId8" xr:uid="{268C4708-7DC2-314B-9749-796D12F7E880}"/>
-    <hyperlink ref="F16" r:id="rId9" xr:uid="{29CA4407-45EB-BB41-BD80-2829DD24604B}"/>
-    <hyperlink ref="F17" r:id="rId10" xr:uid="{43B53690-B17A-A44B-81C3-40F7FD89E575}"/>
-    <hyperlink ref="F18" r:id="rId11" xr:uid="{A2B24F3C-7C75-9648-9F50-2DFF415C57E9}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{A264EE7C-CB8A-F347-BAFA-CFDFCAB22BEE}"/>
-    <hyperlink ref="F4" r:id="rId13" xr:uid="{104469C6-496F-EC4F-A7AB-D10705F8150E}"/>
-    <hyperlink ref="F5" r:id="rId14" xr:uid="{A5943F82-177A-AC4C-B541-DBD1B68C3C0A}"/>
-    <hyperlink ref="F6" r:id="rId15" xr:uid="{EB150305-E1F8-9D4F-B1B4-376A9B89555A}"/>
-    <hyperlink ref="F7" r:id="rId16" xr:uid="{ADBB449F-89CB-B241-9EB7-739EEEF97803}"/>
-    <hyperlink ref="F8" r:id="rId17" xr:uid="{C402538B-E213-5E4D-A98B-0C5CCD007ADC}"/>
-    <hyperlink ref="F2" r:id="rId18" xr:uid="{836CF848-D4B9-FE47-9961-ED6DA8418687}"/>
-    <hyperlink ref="F20" r:id="rId19" xr:uid="{14532B07-9853-C348-857E-7B8B340A8F90}"/>
+    <hyperlink ref="G19" r:id="rId1" xr:uid="{3BC06DD8-1C63-2A4C-8A9E-4A19047DD22C}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{3C89D393-F689-FF47-8088-FFA957C54119}"/>
+    <hyperlink ref="G10" r:id="rId3" xr:uid="{EA3E43BA-BFF4-9C40-B63C-84926F27C27D}"/>
+    <hyperlink ref="G11" r:id="rId4" xr:uid="{171C8763-89F5-7E4F-88BC-7A0EA89B85D5}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{82BD3B5B-C242-4E42-9ABC-C1399D16A6F1}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{A7DE2133-3CE9-094B-9275-BBEBE0F66E3A}"/>
+    <hyperlink ref="G14" r:id="rId7" xr:uid="{31168212-B833-9745-90EB-D87CA8F4357E}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{268C4708-7DC2-314B-9749-796D12F7E880}"/>
+    <hyperlink ref="G16" r:id="rId9" xr:uid="{29CA4407-45EB-BB41-BD80-2829DD24604B}"/>
+    <hyperlink ref="G17" r:id="rId10" xr:uid="{43B53690-B17A-A44B-81C3-40F7FD89E575}"/>
+    <hyperlink ref="G18" r:id="rId11" xr:uid="{A2B24F3C-7C75-9648-9F50-2DFF415C57E9}"/>
+    <hyperlink ref="G3" r:id="rId12" xr:uid="{A264EE7C-CB8A-F347-BAFA-CFDFCAB22BEE}"/>
+    <hyperlink ref="G4" r:id="rId13" xr:uid="{104469C6-496F-EC4F-A7AB-D10705F8150E}"/>
+    <hyperlink ref="G5" r:id="rId14" xr:uid="{A5943F82-177A-AC4C-B541-DBD1B68C3C0A}"/>
+    <hyperlink ref="G6" r:id="rId15" xr:uid="{EB150305-E1F8-9D4F-B1B4-376A9B89555A}"/>
+    <hyperlink ref="G7" r:id="rId16" xr:uid="{ADBB449F-89CB-B241-9EB7-739EEEF97803}"/>
+    <hyperlink ref="G8" r:id="rId17" xr:uid="{C402538B-E213-5E4D-A98B-0C5CCD007ADC}"/>
+    <hyperlink ref="G2" r:id="rId18" xr:uid="{836CF848-D4B9-FE47-9961-ED6DA8418687}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{14532B07-9853-C348-857E-7B8B340A8F90}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{B8E75423-DF77-5E40-8E0F-19D4EBD24616}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId20"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for March 16.
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5520BE-C729-E544-8AF5-823335DF0754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C86F2A-B36D-3A42-9317-42F711712F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{52E8CECD-B562-9649-AE5E-9D9A22BA9B75}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/ontario-new-covid-19-cases-total-sunday-1.5498410</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/ontario-covid-19-coronavirus-monday-1.5498849</t>
   </si>
 </sst>
 </file>
@@ -278,10 +281,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Ontario!$D$2:$D$21</c:f>
+              <c:f>Ontario!$D$2:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -341,16 +344,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Ontario!$B$2:$B$21</c:f>
+              <c:f>Ontario!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -409,7 +415,10 @@
                   <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>145</c:v>
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1284,13 +1293,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1616,7 +1625,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A9237A-1352-3E4D-BF1A-5255317D7F41}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2087,7 +2096,7 @@
         <v>43905</v>
       </c>
       <c r="B21">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C21">
         <v>8465</v>
@@ -2102,10 +2111,36 @@
       </c>
       <c r="F21" s="2">
         <f t="shared" si="1"/>
-        <v>0.40776699029126218</v>
+        <v>0.41747572815533984</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43906</v>
+      </c>
+      <c r="B22">
+        <v>177</v>
+      </c>
+      <c r="C22">
+        <v>10178</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22" si="3">A22-$A$2</f>
+        <v>51</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22" si="4">D22-D21</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" ref="F22" si="5">(B22/B21)^(1/E22)-1</f>
+        <v>0.21232876712328763</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2130,8 +2165,9 @@
     <hyperlink ref="G2" r:id="rId18" xr:uid="{836CF848-D4B9-FE47-9961-ED6DA8418687}"/>
     <hyperlink ref="G20" r:id="rId19" xr:uid="{14532B07-9853-C348-857E-7B8B340A8F90}"/>
     <hyperlink ref="G21" r:id="rId20" xr:uid="{B8E75423-DF77-5E40-8E0F-19D4EBD24616}"/>
+    <hyperlink ref="G22" r:id="rId21" xr:uid="{88193BF4-A4F5-CD49-BE90-9995D3237198}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for March 17 and add automation
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C86F2A-B36D-3A42-9317-42F711712F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{52E8CECD-B562-9649-AE5E-9D9A22BA9B75}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520"/>
   </bookViews>
   <sheets>
-    <sheet name="Ontario" sheetId="1" r:id="rId1"/>
+    <sheet name="OntarioCoronavirus.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -117,12 +114,15 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/ontario-covid-19-coronavirus-monday-1.5498849</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/coronavirus-covid-19-ontario-tuesday-1.5500006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -208,6 +208,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -248,7 +249,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Ontario!$B$1</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -281,150 +282,156 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Ontario!$D$2:$D$22</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>48</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Ontario!$B$2:$B$22</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>79</c:v>
+                  <c:v>79.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>103</c:v>
+                  <c:v>103.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>146</c:v>
+                  <c:v>146.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>177</c:v>
+                  <c:v>177.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>188.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-00DE-CC47-B4C1-885FDDD9C6E5}"/>
             </c:ext>
@@ -438,11 +445,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1367640784"/>
-        <c:axId val="1367642416"/>
+        <c:axId val="2096556056"/>
+        <c:axId val="2096569192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1367640784"/>
+        <c:axId val="2096556056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,6 +499,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -500,26 +508,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -558,12 +546,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1367642416"/>
+        <c:crossAx val="2096569192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1367642416"/>
+        <c:axId val="2096569192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,6 +597,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -617,26 +606,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -675,7 +644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1367640784"/>
+        <c:crossAx val="2096556056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -689,14 +658,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -731,575 +700,19 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1307,7 +720,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1371,7 +784,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1423,7 +836,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1617,19 +1030,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A9237A-1352-3E4D-BF1A-5255317D7F41}">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
@@ -1639,7 +1054,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1662,7 +1077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>43855</v>
       </c>
@@ -1677,7 +1092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>43857</v>
       </c>
@@ -1700,7 +1115,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>43861</v>
       </c>
@@ -1723,7 +1138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>43884</v>
       </c>
@@ -1746,7 +1161,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>43887</v>
       </c>
@@ -1769,7 +1184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>43888</v>
       </c>
@@ -1792,7 +1207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>43889</v>
       </c>
@@ -1815,7 +1230,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>43890</v>
       </c>
@@ -1838,7 +1253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>43891</v>
       </c>
@@ -1861,7 +1276,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -1884,7 +1299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>43893</v>
       </c>
@@ -1907,7 +1322,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>43895</v>
       </c>
@@ -1930,7 +1345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>43896</v>
       </c>
@@ -1953,7 +1368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
@@ -1976,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>43900</v>
       </c>
@@ -1999,7 +1414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>43901</v>
       </c>
@@ -2022,7 +1437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>43902</v>
       </c>
@@ -2045,7 +1460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>43903</v>
       </c>
@@ -2068,7 +1483,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>43904</v>
       </c>
@@ -2091,7 +1506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>43905</v>
       </c>
@@ -2117,7 +1532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>43906</v>
       </c>
@@ -2143,31 +1558,64 @@
         <v>27</v>
       </c>
     </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1">
+        <v>43907</v>
+      </c>
+      <c r="B23">
+        <v>188</v>
+      </c>
+      <c r="C23">
+        <v>11171</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23" si="6">A23-$A$2</f>
+        <v>52</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23" si="7">D23-D22</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" ref="F23" si="8">(B23/B22)^(1/E23)-1</f>
+        <v>6.2146892655367214E-2</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1" xr:uid="{3BC06DD8-1C63-2A4C-8A9E-4A19047DD22C}"/>
-    <hyperlink ref="G9" r:id="rId2" xr:uid="{3C89D393-F689-FF47-8088-FFA957C54119}"/>
-    <hyperlink ref="G10" r:id="rId3" xr:uid="{EA3E43BA-BFF4-9C40-B63C-84926F27C27D}"/>
-    <hyperlink ref="G11" r:id="rId4" xr:uid="{171C8763-89F5-7E4F-88BC-7A0EA89B85D5}"/>
-    <hyperlink ref="G12" r:id="rId5" xr:uid="{82BD3B5B-C242-4E42-9ABC-C1399D16A6F1}"/>
-    <hyperlink ref="G13" r:id="rId6" xr:uid="{A7DE2133-3CE9-094B-9275-BBEBE0F66E3A}"/>
-    <hyperlink ref="G14" r:id="rId7" xr:uid="{31168212-B833-9745-90EB-D87CA8F4357E}"/>
-    <hyperlink ref="G15" r:id="rId8" xr:uid="{268C4708-7DC2-314B-9749-796D12F7E880}"/>
-    <hyperlink ref="G16" r:id="rId9" xr:uid="{29CA4407-45EB-BB41-BD80-2829DD24604B}"/>
-    <hyperlink ref="G17" r:id="rId10" xr:uid="{43B53690-B17A-A44B-81C3-40F7FD89E575}"/>
-    <hyperlink ref="G18" r:id="rId11" xr:uid="{A2B24F3C-7C75-9648-9F50-2DFF415C57E9}"/>
-    <hyperlink ref="G3" r:id="rId12" xr:uid="{A264EE7C-CB8A-F347-BAFA-CFDFCAB22BEE}"/>
-    <hyperlink ref="G4" r:id="rId13" xr:uid="{104469C6-496F-EC4F-A7AB-D10705F8150E}"/>
-    <hyperlink ref="G5" r:id="rId14" xr:uid="{A5943F82-177A-AC4C-B541-DBD1B68C3C0A}"/>
-    <hyperlink ref="G6" r:id="rId15" xr:uid="{EB150305-E1F8-9D4F-B1B4-376A9B89555A}"/>
-    <hyperlink ref="G7" r:id="rId16" xr:uid="{ADBB449F-89CB-B241-9EB7-739EEEF97803}"/>
-    <hyperlink ref="G8" r:id="rId17" xr:uid="{C402538B-E213-5E4D-A98B-0C5CCD007ADC}"/>
-    <hyperlink ref="G2" r:id="rId18" xr:uid="{836CF848-D4B9-FE47-9961-ED6DA8418687}"/>
-    <hyperlink ref="G20" r:id="rId19" xr:uid="{14532B07-9853-C348-857E-7B8B340A8F90}"/>
-    <hyperlink ref="G21" r:id="rId20" xr:uid="{B8E75423-DF77-5E40-8E0F-19D4EBD24616}"/>
-    <hyperlink ref="G22" r:id="rId21" xr:uid="{88193BF4-A4F5-CD49-BE90-9995D3237198}"/>
+    <hyperlink ref="G19" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G11" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="G13" r:id="rId6"/>
+    <hyperlink ref="G14" r:id="rId7"/>
+    <hyperlink ref="G15" r:id="rId8"/>
+    <hyperlink ref="G16" r:id="rId9"/>
+    <hyperlink ref="G17" r:id="rId10"/>
+    <hyperlink ref="G18" r:id="rId11"/>
+    <hyperlink ref="G3" r:id="rId12"/>
+    <hyperlink ref="G4" r:id="rId13"/>
+    <hyperlink ref="G5" r:id="rId14"/>
+    <hyperlink ref="G6" r:id="rId15"/>
+    <hyperlink ref="G7" r:id="rId16"/>
+    <hyperlink ref="G8" r:id="rId17"/>
+    <hyperlink ref="G2" r:id="rId18"/>
+    <hyperlink ref="G20" r:id="rId19"/>
+    <hyperlink ref="G21" r:id="rId20"/>
+    <hyperlink ref="G22" r:id="rId21"/>
+    <hyperlink ref="G23" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId23"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for March 18
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="OntarioCoronavirus.csv" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/coronavirus-covid-19-ontario-tuesday-1.5500006</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/coronavirus-covid-19-ontario-wednesday-1.5501250</t>
   </si>
 </sst>
 </file>
@@ -282,10 +285,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$23</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -351,16 +354,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$23</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -426,6 +432,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>188.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>212.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -706,13 +715,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1038,11 +1047,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1569,19 +1576,45 @@
         <v>11171</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23" si="6">A23-$A$2</f>
+        <f t="shared" ref="D23:D24" si="6">A23-$A$2</f>
         <v>52</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23" si="7">D23-D22</f>
+        <f t="shared" ref="E23:E24" si="7">D23-D22</f>
         <v>1</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" ref="F23" si="8">(B23/B22)^(1/E23)-1</f>
+        <f t="shared" ref="F23:F24" si="8">(B23/B22)^(1/E23)-1</f>
         <v>6.2146892655367214E-2</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B24">
+        <v>212</v>
+      </c>
+      <c r="C24">
+        <v>13897</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="6"/>
+        <v>53</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="8"/>
+        <v>0.12765957446808507</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1608,10 +1641,11 @@
     <hyperlink ref="G21" r:id="rId20"/>
     <hyperlink ref="G22" r:id="rId21"/>
     <hyperlink ref="G23" r:id="rId22"/>
+    <hyperlink ref="G24" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId23"/>
+  <drawing r:id="rId24"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for March 19
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590D7D10-BD46-4645-B59A-131423D0909E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OntarioCoronavirus.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,12 +28,15 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -120,12 +126,15 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/coronavirus-covid-19-ontario-wednesday-1.5501250</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/coronavirus-covid-19-ontario-thursday-emergency-bill-1.5502527</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -197,7 +206,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -211,7 +220,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -290,73 +298,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51.0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>52.0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>53.0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -368,79 +376,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>79.0</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>103.0</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>146.0</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>177.0</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>188.0</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>212.0</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-00DE-CC47-B4C1-885FDDD9C6E5}"/>
             </c:ext>
@@ -508,7 +516,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -606,7 +613,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -667,14 +673,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -715,13 +721,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -729,7 +735,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1039,19 +1045,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
@@ -1061,7 +1069,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43855</v>
       </c>
@@ -1099,7 +1107,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43857</v>
       </c>
@@ -1122,7 +1130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43861</v>
       </c>
@@ -1145,7 +1153,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43884</v>
       </c>
@@ -1168,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43887</v>
       </c>
@@ -1191,7 +1199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43888</v>
       </c>
@@ -1214,7 +1222,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43889</v>
       </c>
@@ -1237,7 +1245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43890</v>
       </c>
@@ -1260,7 +1268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43891</v>
       </c>
@@ -1283,7 +1291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -1306,7 +1314,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43893</v>
       </c>
@@ -1329,7 +1337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43895</v>
       </c>
@@ -1352,7 +1360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43896</v>
       </c>
@@ -1375,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
@@ -1398,7 +1406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43900</v>
       </c>
@@ -1421,7 +1429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43901</v>
       </c>
@@ -1444,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43902</v>
       </c>
@@ -1467,7 +1475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43903</v>
       </c>
@@ -1490,7 +1498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43904</v>
       </c>
@@ -1513,7 +1521,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43905</v>
       </c>
@@ -1539,7 +1547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43906</v>
       </c>
@@ -1565,7 +1573,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43907</v>
       </c>
@@ -1576,7 +1584,7 @@
         <v>11171</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D24" si="6">A23-$A$2</f>
+        <f t="shared" ref="D23:D25" si="6">A23-$A$2</f>
         <v>52</v>
       </c>
       <c r="E23">
@@ -1591,12 +1599,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43908</v>
       </c>
       <c r="B24">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C24">
         <v>13897</v>
@@ -1611,41 +1619,68 @@
       </c>
       <c r="F24" s="2">
         <f t="shared" si="8"/>
-        <v>0.12765957446808507</v>
+        <v>0.13829787234042556</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43909</v>
+      </c>
+      <c r="B25">
+        <v>258</v>
+      </c>
+      <c r="C25">
+        <v>16650</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25" si="9">D25-D24</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25" si="10">(B25/B24)^(1/E25)-1</f>
+        <v>0.20560747663551404</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1"/>
-    <hyperlink ref="G9" r:id="rId2"/>
-    <hyperlink ref="G10" r:id="rId3"/>
-    <hyperlink ref="G11" r:id="rId4"/>
-    <hyperlink ref="G12" r:id="rId5"/>
-    <hyperlink ref="G13" r:id="rId6"/>
-    <hyperlink ref="G14" r:id="rId7"/>
-    <hyperlink ref="G15" r:id="rId8"/>
-    <hyperlink ref="G16" r:id="rId9"/>
-    <hyperlink ref="G17" r:id="rId10"/>
-    <hyperlink ref="G18" r:id="rId11"/>
-    <hyperlink ref="G3" r:id="rId12"/>
-    <hyperlink ref="G4" r:id="rId13"/>
-    <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G6" r:id="rId15"/>
-    <hyperlink ref="G7" r:id="rId16"/>
-    <hyperlink ref="G8" r:id="rId17"/>
-    <hyperlink ref="G2" r:id="rId18"/>
-    <hyperlink ref="G20" r:id="rId19"/>
-    <hyperlink ref="G21" r:id="rId20"/>
-    <hyperlink ref="G22" r:id="rId21"/>
-    <hyperlink ref="G23" r:id="rId22"/>
-    <hyperlink ref="G24" r:id="rId23"/>
+    <hyperlink ref="G19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G3" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G5" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G7" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G8" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G25" r:id="rId24" xr:uid="{FDA1CC55-4C7E-ED4E-AE7C-185C199BB505}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId24"/>
+  <drawing r:id="rId25"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for March 20
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590D7D10-BD46-4645-B59A-131423D0909E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65914D37-8F3E-A24C-A56A-D95055321B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/coronavirus-covid-19-ontario-thursday-emergency-bill-1.5502527</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/coronavirus-covid-19-ontario-friday-online-learning-1.5504109</t>
   </si>
 </sst>
 </file>
@@ -293,10 +296,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$24</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -365,16 +368,22 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$24</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -443,6 +452,12 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>318</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -721,13 +736,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -799,7 +814,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -851,7 +866,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1053,11 +1068,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1584,7 +1597,7 @@
         <v>11171</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D25" si="6">A23-$A$2</f>
+        <f t="shared" ref="D23:D26" si="6">A23-$A$2</f>
         <v>52</v>
       </c>
       <c r="E23">
@@ -1649,6 +1662,32 @@
       </c>
       <c r="G25" s="3" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43910</v>
+      </c>
+      <c r="B26">
+        <v>318</v>
+      </c>
+      <c r="C26">
+        <v>19511</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26" si="11">D26-D25</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" ref="F26" si="12">(B26/B25)^(1/E26)-1</f>
+        <v>0.23255813953488369</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1677,10 +1716,11 @@
     <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="G25" r:id="rId24" xr:uid="{FDA1CC55-4C7E-ED4E-AE7C-185C199BB505}"/>
+    <hyperlink ref="G26" r:id="rId25" xr:uid="{C9E1F4D2-3947-3C45-B25D-405B5174D1BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId25"/>
+  <drawing r:id="rId26"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for March 21
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65914D37-8F3E-A24C-A56A-D95055321B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AB5F4E-C602-FE4C-B3CF-50B48A78D49E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/coronavirus-covid-19-ontario-friday-online-learning-1.5504109</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/ontario-hospital-association-pleads-for-social-distancing-1.5505827</t>
   </si>
 </sst>
 </file>
@@ -296,10 +299,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$26</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -374,16 +377,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$26</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -458,6 +464,9 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -736,13 +745,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1068,7 +1077,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1597,7 +1606,7 @@
         <v>11171</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D26" si="6">A23-$A$2</f>
+        <f t="shared" ref="D23:D27" si="6">A23-$A$2</f>
         <v>52</v>
       </c>
       <c r="E23">
@@ -1688,6 +1697,32 @@
       </c>
       <c r="G26" s="3" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>43911</v>
+      </c>
+      <c r="B27">
+        <v>377</v>
+      </c>
+      <c r="C27">
+        <v>23384</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="6"/>
+        <v>56</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27" si="13">D27-D26</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" ref="F27" si="14">(B27/B26)^(1/E27)-1</f>
+        <v>0.18553459119496862</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1717,10 +1752,11 @@
     <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="G25" r:id="rId24" xr:uid="{FDA1CC55-4C7E-ED4E-AE7C-185C199BB505}"/>
     <hyperlink ref="G26" r:id="rId25" xr:uid="{C9E1F4D2-3947-3C45-B25D-405B5174D1BB}"/>
+    <hyperlink ref="G27" r:id="rId26" xr:uid="{55B92E3A-A221-0D43-BA4B-9AAC89C8B827}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId26"/>
+  <drawing r:id="rId27"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for March 22
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AB5F4E-C602-FE4C-B3CF-50B48A78D49E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C57FE1-91DA-954C-A2E5-E859E7201342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/ontario-hospital-association-pleads-for-social-distancing-1.5505827</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/ontario-hospital-powers-redeploy-staff-covid-19-1.5506052</t>
   </si>
 </sst>
 </file>
@@ -299,10 +302,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$27</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -380,16 +383,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$27</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -467,6 +473,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -745,13 +754,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1077,7 +1086,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1723,6 +1732,32 @@
       </c>
       <c r="G27" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B28">
+        <v>424</v>
+      </c>
+      <c r="C28">
+        <v>26420</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28" si="15">A28-$A$2</f>
+        <v>57</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28" si="16">D28-D27</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" ref="F28" si="17">(B28/B27)^(1/E28)-1</f>
+        <v>0.12466843501326252</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1753,10 +1788,11 @@
     <hyperlink ref="G25" r:id="rId24" xr:uid="{FDA1CC55-4C7E-ED4E-AE7C-185C199BB505}"/>
     <hyperlink ref="G26" r:id="rId25" xr:uid="{C9E1F4D2-3947-3C45-B25D-405B5174D1BB}"/>
     <hyperlink ref="G27" r:id="rId26" xr:uid="{55B92E3A-A221-0D43-BA4B-9AAC89C8B827}"/>
+    <hyperlink ref="G28" r:id="rId27" xr:uid="{6AE0AFBD-3407-9F47-B4AC-A9743D420238}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId27"/>
+  <drawing r:id="rId28"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for March 23
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C57FE1-91DA-954C-A2E5-E859E7201342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="OntarioCoronavirus.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,15 +25,12 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -138,12 +132,15 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/ontario-hospital-powers-redeploy-staff-covid-19-1.5506052</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-ontario-monday-1.5506445</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -215,7 +212,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -229,6 +226,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -302,186 +300,192 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$28</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>48</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>53</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>54</c:v>
+                  <c:v>54.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>55</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>56</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>57</c:v>
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>58.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$28</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>79</c:v>
+                  <c:v>79.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>103</c:v>
+                  <c:v>103.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>146</c:v>
+                  <c:v>146.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>177</c:v>
+                  <c:v>177.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>188</c:v>
+                  <c:v>188.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>214</c:v>
+                  <c:v>214.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>258</c:v>
+                  <c:v>258.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>318</c:v>
+                  <c:v>318.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>377</c:v>
+                  <c:v>377.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>424</c:v>
+                  <c:v>424.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>503.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-00DE-CC47-B4C1-885FDDD9C6E5}"/>
             </c:ext>
@@ -495,11 +499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2096556056"/>
-        <c:axId val="2096569192"/>
+        <c:axId val="2118386392"/>
+        <c:axId val="2093159096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2096556056"/>
+        <c:axId val="2118386392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,6 +553,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -595,12 +600,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096569192"/>
+        <c:crossAx val="2093159096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2096569192"/>
+        <c:axId val="2093159096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,6 +651,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -692,7 +698,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096556056"/>
+        <c:crossAx val="2118386392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -706,14 +712,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -754,13 +760,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -768,7 +774,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -832,7 +838,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -884,7 +890,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1078,19 +1084,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
@@ -1100,7 +1106,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>43855</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>43857</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>43861</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>43884</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>43887</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>43888</v>
       </c>
@@ -1253,7 +1259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>43889</v>
       </c>
@@ -1276,7 +1282,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>43890</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>43891</v>
       </c>
@@ -1322,7 +1328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -1345,7 +1351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>43893</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>43895</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>43896</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
@@ -1437,7 +1443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>43900</v>
       </c>
@@ -1460,7 +1466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>43901</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>43902</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>43903</v>
       </c>
@@ -1529,7 +1535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>43904</v>
       </c>
@@ -1552,7 +1558,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>43905</v>
       </c>
@@ -1578,7 +1584,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>43906</v>
       </c>
@@ -1604,7 +1610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>43907</v>
       </c>
@@ -1630,7 +1636,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>43908</v>
       </c>
@@ -1656,7 +1662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>43909</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>43910</v>
       </c>
@@ -1708,7 +1714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>43911</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>43912</v>
       </c>
@@ -1745,54 +1751,81 @@
         <v>26420</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28" si="15">A28-$A$2</f>
+        <f t="shared" ref="D28:D29" si="15">A28-$A$2</f>
         <v>57</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28" si="16">D28-D27</f>
+        <f t="shared" ref="E28:E29" si="16">D28-D27</f>
         <v>1</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" ref="F28" si="17">(B28/B27)^(1/E28)-1</f>
+        <f t="shared" ref="F28:F29" si="17">(B28/B27)^(1/E28)-1</f>
         <v>0.12466843501326252</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B29">
+        <v>503</v>
+      </c>
+      <c r="C29">
+        <v>28506</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="15"/>
+        <v>58</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="17"/>
+        <v>0.18632075471698117</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G3" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G5" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G7" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G8" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G25" r:id="rId24" xr:uid="{FDA1CC55-4C7E-ED4E-AE7C-185C199BB505}"/>
-    <hyperlink ref="G26" r:id="rId25" xr:uid="{C9E1F4D2-3947-3C45-B25D-405B5174D1BB}"/>
-    <hyperlink ref="G27" r:id="rId26" xr:uid="{55B92E3A-A221-0D43-BA4B-9AAC89C8B827}"/>
-    <hyperlink ref="G28" r:id="rId27" xr:uid="{6AE0AFBD-3407-9F47-B4AC-A9743D420238}"/>
+    <hyperlink ref="G19" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G11" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="G13" r:id="rId6"/>
+    <hyperlink ref="G14" r:id="rId7"/>
+    <hyperlink ref="G15" r:id="rId8"/>
+    <hyperlink ref="G16" r:id="rId9"/>
+    <hyperlink ref="G17" r:id="rId10"/>
+    <hyperlink ref="G18" r:id="rId11"/>
+    <hyperlink ref="G3" r:id="rId12"/>
+    <hyperlink ref="G4" r:id="rId13"/>
+    <hyperlink ref="G5" r:id="rId14"/>
+    <hyperlink ref="G6" r:id="rId15"/>
+    <hyperlink ref="G7" r:id="rId16"/>
+    <hyperlink ref="G8" r:id="rId17"/>
+    <hyperlink ref="G2" r:id="rId18"/>
+    <hyperlink ref="G20" r:id="rId19"/>
+    <hyperlink ref="G21" r:id="rId20"/>
+    <hyperlink ref="G22" r:id="rId21"/>
+    <hyperlink ref="G23" r:id="rId22"/>
+    <hyperlink ref="G24" r:id="rId23"/>
+    <hyperlink ref="G25" r:id="rId24"/>
+    <hyperlink ref="G26" r:id="rId25"/>
+    <hyperlink ref="G27" r:id="rId26"/>
+    <hyperlink ref="G28" r:id="rId27"/>
+    <hyperlink ref="G29" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId28"/>
+  <drawing r:id="rId29"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for March 24
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-ontario-monday-1.5506445</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-ontario-tuesday-hydro-1.5507767</t>
   </si>
 </sst>
 </file>
@@ -300,10 +303,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$29</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -387,16 +390,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>59.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$29</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -480,6 +486,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>503.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>588.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -760,13 +769,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1092,7 +1101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1790,6 +1799,32 @@
       </c>
       <c r="G29" s="3" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B30">
+        <v>588</v>
+      </c>
+      <c r="C30">
+        <v>32457</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30" si="18">A30-$A$2</f>
+        <v>59</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ref="E30" si="19">D30-D29</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" ref="F30" si="20">(B30/B29)^(1/E30)-1</f>
+        <v>0.16898608349900601</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1822,10 +1857,11 @@
     <hyperlink ref="G27" r:id="rId26"/>
     <hyperlink ref="G28" r:id="rId27"/>
     <hyperlink ref="G29" r:id="rId28"/>
+    <hyperlink ref="G30" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId29"/>
+  <drawing r:id="rId30"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for March 26
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294EC87F-6D74-5147-BC0E-A87606D8A818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OntarioCoronavirus.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,12 +28,15 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -107,9 +113,6 @@
     <t>https://www.cbc.ca/news/canada/toronto/toronto-covid-19-march-14-1.5497959</t>
   </si>
   <si>
-    <t>Tests Conducted</t>
-  </si>
-  <si>
     <t>https://www.cbc.ca/news/canada/toronto/ontario-new-covid-19-cases-total-sunday-1.5498410</t>
   </si>
   <si>
@@ -138,12 +141,21 @@
   </si>
   <si>
     <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-ontario-tuesday-hydro-1.5507767</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-thursday-new-cases-1.5510534</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-wednesday-fiscal-outlook-1.5509193</t>
+  </si>
+  <si>
+    <t>Tests Approved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -215,7 +227,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -229,7 +241,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -303,198 +314,210 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$30</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51.0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>52.0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>53.0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>54.0</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>57.0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>58.0</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>59.0</c:v>
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$30</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>79.0</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>103.0</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>146.0</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>177.0</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>188.0</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>214.0</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>258.0</c:v>
+                  <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>318.0</c:v>
+                  <c:v>318</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>377.0</c:v>
+                  <c:v>377</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>424.0</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>503.0</c:v>
+                  <c:v>503</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>588.0</c:v>
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>688</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>858</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-00DE-CC47-B4C1-885FDDD9C6E5}"/>
             </c:ext>
@@ -562,7 +585,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -660,7 +682,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -721,14 +742,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -769,13 +790,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -783,7 +804,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1093,19 +1114,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
@@ -1115,7 +1136,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1144,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1138,7 +1159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43855</v>
       </c>
@@ -1153,7 +1174,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43857</v>
       </c>
@@ -1176,7 +1197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43861</v>
       </c>
@@ -1199,7 +1220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43884</v>
       </c>
@@ -1222,7 +1243,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43887</v>
       </c>
@@ -1245,7 +1266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43888</v>
       </c>
@@ -1268,7 +1289,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43889</v>
       </c>
@@ -1291,7 +1312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43890</v>
       </c>
@@ -1314,7 +1335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43891</v>
       </c>
@@ -1337,7 +1358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -1360,7 +1381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43893</v>
       </c>
@@ -1383,7 +1404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43895</v>
       </c>
@@ -1406,7 +1427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43896</v>
       </c>
@@ -1429,7 +1450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
@@ -1452,7 +1473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43900</v>
       </c>
@@ -1475,7 +1496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43901</v>
       </c>
@@ -1498,7 +1519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43902</v>
       </c>
@@ -1521,7 +1542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43903</v>
       </c>
@@ -1544,7 +1565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43904</v>
       </c>
@@ -1567,7 +1588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43905</v>
       </c>
@@ -1590,10 +1611,10 @@
         <v>0.41747572815533984</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43906</v>
       </c>
@@ -1616,10 +1637,10 @@
         <v>0.21232876712328763</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43907</v>
       </c>
@@ -1642,10 +1663,10 @@
         <v>6.2146892655367214E-2</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43908</v>
       </c>
@@ -1668,10 +1689,10 @@
         <v>0.13829787234042556</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43909</v>
       </c>
@@ -1694,10 +1715,10 @@
         <v>0.20560747663551404</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43910</v>
       </c>
@@ -1720,10 +1741,10 @@
         <v>0.23255813953488369</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43911</v>
       </c>
@@ -1746,10 +1767,10 @@
         <v>0.18553459119496862</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43912</v>
       </c>
@@ -1772,10 +1793,10 @@
         <v>0.12466843501326252</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43913</v>
       </c>
@@ -1798,10 +1819,10 @@
         <v>0.18632075471698117</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43914</v>
       </c>
@@ -1812,56 +1833,110 @@
         <v>32457</v>
       </c>
       <c r="D30">
-        <f t="shared" ref="D30" si="18">A30-$A$2</f>
+        <f>A30-$A$2</f>
         <v>59</v>
       </c>
       <c r="E30">
-        <f t="shared" ref="E30" si="19">D30-D29</f>
+        <f>D30-D29</f>
         <v>1</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" ref="F30" si="20">(B30/B29)^(1/E30)-1</f>
+        <f t="shared" ref="F30" si="18">(B30/B29)^(1/E30)-1</f>
         <v>0.16898608349900601</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B31">
+        <v>688</v>
+      </c>
+      <c r="C31">
+        <v>35635</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:D32" si="19">A31-$A$2</f>
+        <v>60</v>
+      </c>
+      <c r="E31">
+        <f>D31-D30</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" ref="F31:F32" si="20">(B31/B30)^(1/E31)-1</f>
+        <v>0.17006802721088432</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B32">
+        <v>858</v>
+      </c>
+      <c r="C32">
+        <v>38550</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="19"/>
+        <v>61</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ref="E31:E32" si="21">D32-D31</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="20"/>
+        <v>0.24709302325581395</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1"/>
-    <hyperlink ref="G9" r:id="rId2"/>
-    <hyperlink ref="G10" r:id="rId3"/>
-    <hyperlink ref="G11" r:id="rId4"/>
-    <hyperlink ref="G12" r:id="rId5"/>
-    <hyperlink ref="G13" r:id="rId6"/>
-    <hyperlink ref="G14" r:id="rId7"/>
-    <hyperlink ref="G15" r:id="rId8"/>
-    <hyperlink ref="G16" r:id="rId9"/>
-    <hyperlink ref="G17" r:id="rId10"/>
-    <hyperlink ref="G18" r:id="rId11"/>
-    <hyperlink ref="G3" r:id="rId12"/>
-    <hyperlink ref="G4" r:id="rId13"/>
-    <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G6" r:id="rId15"/>
-    <hyperlink ref="G7" r:id="rId16"/>
-    <hyperlink ref="G8" r:id="rId17"/>
-    <hyperlink ref="G2" r:id="rId18"/>
-    <hyperlink ref="G20" r:id="rId19"/>
-    <hyperlink ref="G21" r:id="rId20"/>
-    <hyperlink ref="G22" r:id="rId21"/>
-    <hyperlink ref="G23" r:id="rId22"/>
-    <hyperlink ref="G24" r:id="rId23"/>
-    <hyperlink ref="G25" r:id="rId24"/>
-    <hyperlink ref="G26" r:id="rId25"/>
-    <hyperlink ref="G27" r:id="rId26"/>
-    <hyperlink ref="G28" r:id="rId27"/>
-    <hyperlink ref="G29" r:id="rId28"/>
-    <hyperlink ref="G30" r:id="rId29"/>
+    <hyperlink ref="G19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G3" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G5" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G7" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G8" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G32" r:id="rId30" xr:uid="{C2E5F225-BC07-5247-ABA7-2767C9456B6E}"/>
+    <hyperlink ref="G31" r:id="rId31" xr:uid="{E3B3CDD3-9455-0948-BDB1-AC6E81E361DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId30"/>
+  <drawing r:id="rId32"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for March 27
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanwang/Desktop/OntarioCoronavirus/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294EC87F-6D74-5147-BC0E-A87606D8A818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="OntarioCoronavirus.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,15 +25,12 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -150,12 +144,15 @@
   </si>
   <si>
     <t>Tests Approved</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-friday-lcbo-1.5512014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -227,7 +224,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -241,6 +238,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -314,210 +312,216 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$32</c:f>
+              <c:f>OntarioCoronavirus.csv!$D$2:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>48</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>53</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>54</c:v>
+                  <c:v>54.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>55</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>56</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>57</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>58</c:v>
+                  <c:v>58.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>59</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>61</c:v>
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$32</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>79</c:v>
+                  <c:v>79.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>103</c:v>
+                  <c:v>103.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>146</c:v>
+                  <c:v>146.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>177</c:v>
+                  <c:v>177.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>188</c:v>
+                  <c:v>188.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>214</c:v>
+                  <c:v>214.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>258</c:v>
+                  <c:v>258.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>318</c:v>
+                  <c:v>318.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>377</c:v>
+                  <c:v>377.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>424</c:v>
+                  <c:v>424.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>503</c:v>
+                  <c:v>503.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>588</c:v>
+                  <c:v>588.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>688</c:v>
+                  <c:v>688.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>858</c:v>
+                  <c:v>858.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>993.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-00DE-CC47-B4C1-885FDDD9C6E5}"/>
             </c:ext>
@@ -531,11 +535,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2118386392"/>
-        <c:axId val="2093159096"/>
+        <c:axId val="2095416568"/>
+        <c:axId val="2095400504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2118386392"/>
+        <c:axId val="2095416568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,6 +589,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -631,12 +636,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093159096"/>
+        <c:crossAx val="2095400504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2093159096"/>
+        <c:axId val="2095400504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -682,6 +687,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -728,7 +734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118386392"/>
+        <c:crossAx val="2095416568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -742,14 +748,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -790,13 +796,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -804,7 +810,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1114,19 +1120,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
@@ -1136,7 +1142,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>43855</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>43857</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>43861</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>43884</v>
       </c>
@@ -1243,7 +1249,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>43887</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>43888</v>
       </c>
@@ -1289,7 +1295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>43889</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>43890</v>
       </c>
@@ -1335,7 +1341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>43891</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -1381,7 +1387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>43893</v>
       </c>
@@ -1404,7 +1410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>43895</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>43896</v>
       </c>
@@ -1450,7 +1456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
@@ -1473,7 +1479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>43900</v>
       </c>
@@ -1496,7 +1502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>43901</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>43902</v>
       </c>
@@ -1542,7 +1548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>43903</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>43904</v>
       </c>
@@ -1588,7 +1594,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>43905</v>
       </c>
@@ -1614,7 +1620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>43906</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>43907</v>
       </c>
@@ -1666,7 +1672,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>43908</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>43909</v>
       </c>
@@ -1718,7 +1724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>43910</v>
       </c>
@@ -1744,7 +1750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>43911</v>
       </c>
@@ -1770,7 +1776,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>43912</v>
       </c>
@@ -1796,7 +1802,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>43913</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>43914</v>
       </c>
@@ -1848,7 +1854,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>43915</v>
       </c>
@@ -1859,7 +1865,7 @@
         <v>35635</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D32" si="19">A31-$A$2</f>
+        <f t="shared" ref="D31:D33" si="19">A31-$A$2</f>
         <v>60</v>
       </c>
       <c r="E31">
@@ -1867,14 +1873,14 @@
         <v>1</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" ref="F31:F32" si="20">(B31/B30)^(1/E31)-1</f>
+        <f t="shared" ref="F31:F33" si="20">(B31/B30)^(1/E31)-1</f>
         <v>0.17006802721088432</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>43916</v>
       </c>
@@ -1889,7 +1895,7 @@
         <v>61</v>
       </c>
       <c r="E32">
-        <f t="shared" ref="E31:E32" si="21">D32-D31</f>
+        <f t="shared" ref="E32:E33" si="21">D32-D31</f>
         <v>1</v>
       </c>
       <c r="F32" s="2">
@@ -1900,43 +1906,70 @@
         <v>35</v>
       </c>
     </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B33">
+        <v>993</v>
+      </c>
+      <c r="C33">
+        <v>41032</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="19"/>
+        <v>62</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="20"/>
+        <v>0.15734265734265729</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G3" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G5" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G7" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G8" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G32" r:id="rId30" xr:uid="{C2E5F225-BC07-5247-ABA7-2767C9456B6E}"/>
-    <hyperlink ref="G31" r:id="rId31" xr:uid="{E3B3CDD3-9455-0948-BDB1-AC6E81E361DC}"/>
+    <hyperlink ref="G19" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G11" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="G13" r:id="rId6"/>
+    <hyperlink ref="G14" r:id="rId7"/>
+    <hyperlink ref="G15" r:id="rId8"/>
+    <hyperlink ref="G16" r:id="rId9"/>
+    <hyperlink ref="G17" r:id="rId10"/>
+    <hyperlink ref="G18" r:id="rId11"/>
+    <hyperlink ref="G3" r:id="rId12"/>
+    <hyperlink ref="G4" r:id="rId13"/>
+    <hyperlink ref="G5" r:id="rId14"/>
+    <hyperlink ref="G6" r:id="rId15"/>
+    <hyperlink ref="G7" r:id="rId16"/>
+    <hyperlink ref="G8" r:id="rId17"/>
+    <hyperlink ref="G2" r:id="rId18"/>
+    <hyperlink ref="G20" r:id="rId19"/>
+    <hyperlink ref="G21" r:id="rId20"/>
+    <hyperlink ref="G22" r:id="rId21"/>
+    <hyperlink ref="G23" r:id="rId22"/>
+    <hyperlink ref="G24" r:id="rId23"/>
+    <hyperlink ref="G25" r:id="rId24"/>
+    <hyperlink ref="G26" r:id="rId25"/>
+    <hyperlink ref="G27" r:id="rId26"/>
+    <hyperlink ref="G28" r:id="rId27"/>
+    <hyperlink ref="G29" r:id="rId28"/>
+    <hyperlink ref="G30" r:id="rId29"/>
+    <hyperlink ref="G32" r:id="rId30"/>
+    <hyperlink ref="G31" r:id="rId31"/>
+    <hyperlink ref="G33" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId32"/>
+  <drawing r:id="rId33"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update for April 5
</commit_message>
<xml_diff>
--- a/OntarioCoronavirus.xlsx
+++ b/OntarioCoronavirus.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -143,17 +143,41 @@
     <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-wednesday-fiscal-outlook-1.5509193</t>
   </si>
   <si>
-    <t>Tests Approved</t>
-  </si>
-  <si>
     <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-friday-lcbo-1.5512014</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/ontario-covid-19-april-5-1.5522458</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-ontario-april-4-1.5521962</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-thursday-mental-health-1.5518688</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-friday-models-tests-1.5520192</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-ontario-lecce-schools-1.5515855</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-coronavirus-wednesday-emergency-order-1.5517172</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/covid-19-ontario-emergency-order-march-29-1.5514008</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/151-new-covid-19-cases-in-ontario-as-province-cracks-down-on-price-gouging-large-gatherings-1.5513554</t>
+  </si>
+  <si>
+    <t>https://globalnews.ca/news/6750016/ontario-coronavirus-covid-19-numbers-march-30/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,6 +200,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -194,18 +226,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
@@ -312,10 +349,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$D$2:$D$33</c:f>
+              <c:f>OntarioCoronavirus.csv!$C$2:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -411,16 +448,43 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>71.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OntarioCoronavirus.csv!$B$2:$B$33</c:f>
+              <c:f>OntarioCoronavirus.csv!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -511,11 +575,38 @@
                 <c:pt idx="29">
                   <c:v>688.0</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="30" formatCode="0">
                   <c:v>858.0</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="31" formatCode="0">
                   <c:v>993.0</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0">
+                  <c:v>1144.0</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0">
+                  <c:v>1355.0</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0">
+                  <c:v>1706.0</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0">
+                  <c:v>1966.0</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0">
+                  <c:v>2392.0</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0">
+                  <c:v>2793.0</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0">
+                  <c:v>3255.0</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0">
+                  <c:v>3630.0</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0">
+                  <c:v>4038.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,11 +626,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095416568"/>
-        <c:axId val="2095400504"/>
+        <c:axId val="-2138898072"/>
+        <c:axId val="2146783976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095416568"/>
+        <c:axId val="-2138898072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,12 +727,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095400504"/>
+        <c:crossAx val="2146783976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2095400504"/>
+        <c:axId val="2146783976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,7 +825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095416568"/>
+        <c:crossAx val="-2138898072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -796,13 +887,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -810,7 +901,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28BB367-99B9-D24A-A3AF-2A9910D4779F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1120,7 +1211,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1128,7 +1219,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1136,13 +1227,12 @@
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1150,451 +1240,448 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>43855</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D21" si="0">A2-$A$2</f>
+      <c r="C2">
+        <f>A2-$A$2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>43857</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <f>A3-$A$2</f>
+        <v>2</v>
+      </c>
       <c r="D3">
+        <f>C3-C2</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <f>(B3/B2)^(1/D3)-1</f>
+        <v>0.41421356237309515</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>43861</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>A4-$A$2</f>
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D21" si="0">C4-C3</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <f>(B4/B3)^(1/D4)-1</f>
+        <v>0.1066819197003217</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>43884</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>A5-$A$2</f>
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E5" s="2">
+        <f>(B5/B4)^(1/D5)-1</f>
+        <v>1.2586467339374297E-2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>43887</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>A6-$A$2</f>
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <f>(B6/B5)^(1/D6)-1</f>
+        <v>7.7217345015941907E-2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>43888</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>A7-$A$2</f>
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <f>(B7/B6)^(1/D7)-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>43889</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f>A8-$A$2</f>
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <f>(B8/B7)^(1/D8)-1</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>43890</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <f>A9-$A$2</f>
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <f>(B9/B8)^(1/D9)-1</f>
+        <v>0.375</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <f>A10-$A$2</f>
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <f>(B10/B9)^(1/D10)-1</f>
+        <v>0.36363636363636354</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>43892</v>
+      </c>
+      <c r="B11">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <f>A11-$A$2</f>
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <f>(B11/B10)^(1/D11)-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>43893</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <f>A12-$A$2</f>
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <f>(B12/B11)^(1/D12)-1</f>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>43895</v>
+      </c>
+      <c r="B13">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <f>A13-$A$2</f>
+        <v>40</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E3">
-        <f>D3-D2</f>
-        <v>2</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" ref="F3:F21" si="1">(B3/B2)^(1/E3)-1</f>
-        <v>0.41421356237309515</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>43861</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E21" si="2">D4-D3</f>
-        <v>4</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1066819197003217</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>43884</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" si="1"/>
-        <v>1.2586467339374297E-2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1">
-        <v>43887</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="1"/>
-        <v>7.7217345015941907E-2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1">
-        <v>43888</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1">
-        <v>43889</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333326</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <v>43890</v>
-      </c>
-      <c r="B9">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="1"/>
-        <v>0.375</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1">
-        <v>43891</v>
-      </c>
-      <c r="B10">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="1"/>
-        <v>0.36363636363636354</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>43892</v>
-      </c>
-      <c r="B11">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1">
-        <v>43893</v>
-      </c>
-      <c r="B12">
-        <v>20</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="1"/>
-        <v>0.11111111111111116</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1">
-        <v>43895</v>
-      </c>
-      <c r="B13">
-        <v>23</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="1"/>
+      <c r="E13" s="2">
+        <f>(B13/B12)^(1/D13)-1</f>
         <v>7.2380529476360866E-2</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>43896</v>
       </c>
       <c r="B14">
         <v>28</v>
       </c>
+      <c r="C14">
+        <f>A14-$A$2</f>
+        <v>41</v>
+      </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <f>(B14/B13)^(1/D14)-1</f>
         <v>0.21739130434782616</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
       <c r="B15">
         <v>32</v>
       </c>
+      <c r="C15">
+        <f>A15-$A$2</f>
+        <v>43</v>
+      </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="F15" s="2">
-        <f t="shared" si="1"/>
+      <c r="E15" s="2">
+        <f>(B15/B14)^(1/D15)-1</f>
         <v>6.9044967649697586E-2</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>43900</v>
       </c>
       <c r="B16">
         <v>37</v>
       </c>
+      <c r="C16">
+        <f>A16-$A$2</f>
+        <v>45</v>
+      </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="F16" s="2">
-        <f t="shared" si="1"/>
+      <c r="E16" s="2">
+        <f>(B16/B15)^(1/D16)-1</f>
         <v>7.5290658380328335E-2</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>43901</v>
       </c>
       <c r="B17">
         <v>42</v>
       </c>
+      <c r="C17">
+        <f>A17-$A$2</f>
+        <v>46</v>
+      </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F17" s="2">
-        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <f>(B17/B16)^(1/D17)-1</f>
         <v>0.13513513513513509</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>43902</v>
       </c>
       <c r="B18">
         <v>60</v>
       </c>
+      <c r="C18">
+        <f>A18-$A$2</f>
+        <v>47</v>
+      </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <f>(B18/B17)^(1/D18)-1</f>
         <v>0.4285714285714286</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>43903</v>
       </c>
       <c r="B19">
         <v>79</v>
       </c>
+      <c r="C19">
+        <f>A19-$A$2</f>
+        <v>48</v>
+      </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <f>(B19/B18)^(1/D19)-1</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>43904</v>
       </c>
       <c r="B20">
         <v>103</v>
       </c>
+      <c r="C20">
+        <f>A20-$A$2</f>
+        <v>49</v>
+      </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <f>(B20/B19)^(1/D20)-1</f>
         <v>0.30379746835443044</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>43905</v>
       </c>
@@ -1602,25 +1689,22 @@
         <v>146</v>
       </c>
       <c r="C21">
-        <v>8465</v>
+        <f>A21-$A$2</f>
+        <v>50</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <f>(B21/B20)^(1/D21)-1</f>
         <v>0.41747572815533984</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>43906</v>
       </c>
@@ -1628,25 +1712,22 @@
         <v>177</v>
       </c>
       <c r="C22">
-        <v>10178</v>
+        <f>A22-$A$2</f>
+        <v>51</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22" si="3">A22-$A$2</f>
-        <v>51</v>
-      </c>
-      <c r="E22">
-        <f t="shared" ref="E22" si="4">D22-D21</f>
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" ref="F22" si="5">(B22/B21)^(1/E22)-1</f>
+        <f t="shared" ref="D22" si="1">C22-C21</f>
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <f>(B22/B21)^(1/D22)-1</f>
         <v>0.21232876712328763</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>43907</v>
       </c>
@@ -1654,25 +1735,22 @@
         <v>188</v>
       </c>
       <c r="C23">
-        <v>11171</v>
+        <f>A23-$A$2</f>
+        <v>52</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D27" si="6">A23-$A$2</f>
-        <v>52</v>
-      </c>
-      <c r="E23">
-        <f t="shared" ref="E23:E24" si="7">D23-D22</f>
-        <v>1</v>
-      </c>
-      <c r="F23" s="2">
-        <f t="shared" ref="F23:F24" si="8">(B23/B22)^(1/E23)-1</f>
+        <f t="shared" ref="D23:D24" si="2">C23-C22</f>
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <f>(B23/B22)^(1/D23)-1</f>
         <v>6.2146892655367214E-2</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>43908</v>
       </c>
@@ -1680,25 +1758,22 @@
         <v>214</v>
       </c>
       <c r="C24">
-        <v>13897</v>
+        <f>A24-$A$2</f>
+        <v>53</v>
       </c>
       <c r="D24">
-        <f t="shared" si="6"/>
-        <v>53</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <f>(B24/B23)^(1/D24)-1</f>
         <v>0.13829787234042556</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>43909</v>
       </c>
@@ -1706,25 +1781,22 @@
         <v>258</v>
       </c>
       <c r="C25">
-        <v>16650</v>
+        <f>A25-$A$2</f>
+        <v>54</v>
       </c>
       <c r="D25">
-        <f t="shared" si="6"/>
-        <v>54</v>
-      </c>
-      <c r="E25">
-        <f t="shared" ref="E25" si="9">D25-D24</f>
-        <v>1</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" ref="F25" si="10">(B25/B24)^(1/E25)-1</f>
+        <f t="shared" ref="D25" si="3">C25-C24</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <f>(B25/B24)^(1/D25)-1</f>
         <v>0.20560747663551404</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>43910</v>
       </c>
@@ -1732,25 +1804,22 @@
         <v>318</v>
       </c>
       <c r="C26">
-        <v>19511</v>
+        <f>A26-$A$2</f>
+        <v>55</v>
       </c>
       <c r="D26">
-        <f t="shared" si="6"/>
-        <v>55</v>
-      </c>
-      <c r="E26">
-        <f t="shared" ref="E26" si="11">D26-D25</f>
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
-        <f t="shared" ref="F26" si="12">(B26/B25)^(1/E26)-1</f>
+        <f t="shared" ref="D26" si="4">C26-C25</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <f>(B26/B25)^(1/D26)-1</f>
         <v>0.23255813953488369</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>43911</v>
       </c>
@@ -1758,25 +1827,22 @@
         <v>377</v>
       </c>
       <c r="C27">
-        <v>23384</v>
+        <f>A27-$A$2</f>
+        <v>56</v>
       </c>
       <c r="D27">
-        <f t="shared" si="6"/>
-        <v>56</v>
-      </c>
-      <c r="E27">
-        <f t="shared" ref="E27" si="13">D27-D26</f>
-        <v>1</v>
-      </c>
-      <c r="F27" s="2">
-        <f t="shared" ref="F27" si="14">(B27/B26)^(1/E27)-1</f>
+        <f t="shared" ref="D27" si="5">C27-C26</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <f>(B27/B26)^(1/D27)-1</f>
         <v>0.18553459119496862</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>43912</v>
       </c>
@@ -1784,25 +1850,22 @@
         <v>424</v>
       </c>
       <c r="C28">
-        <v>26420</v>
+        <f>A28-$A$2</f>
+        <v>57</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:D29" si="15">A28-$A$2</f>
-        <v>57</v>
-      </c>
-      <c r="E28">
-        <f t="shared" ref="E28:E29" si="16">D28-D27</f>
-        <v>1</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" ref="F28:F29" si="17">(B28/B27)^(1/E28)-1</f>
+        <f t="shared" ref="D28:D29" si="6">C28-C27</f>
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <f>(B28/B27)^(1/D28)-1</f>
         <v>0.12466843501326252</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>43913</v>
       </c>
@@ -1810,25 +1873,22 @@
         <v>503</v>
       </c>
       <c r="C29">
-        <v>28506</v>
+        <f>A29-$A$2</f>
+        <v>58</v>
       </c>
       <c r="D29">
-        <f t="shared" si="15"/>
-        <v>58</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="F29" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <f>(B29/B28)^(1/D29)-1</f>
         <v>0.18632075471698117</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>43914</v>
       </c>
@@ -1836,25 +1896,22 @@
         <v>588</v>
       </c>
       <c r="C30">
-        <v>32457</v>
-      </c>
-      <c r="D30">
         <f>A30-$A$2</f>
         <v>59</v>
       </c>
-      <c r="E30">
-        <f>D30-D29</f>
-        <v>1</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" ref="F30" si="18">(B30/B29)^(1/E30)-1</f>
+      <c r="D30">
+        <f>C30-C29</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <f>(B30/B29)^(1/D30)-1</f>
         <v>0.16898608349900601</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>43915</v>
       </c>
@@ -1862,114 +1919,321 @@
         <v>688</v>
       </c>
       <c r="C31">
-        <v>35635</v>
+        <f>A31-$A$2</f>
+        <v>60</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D33" si="19">A31-$A$2</f>
-        <v>60</v>
-      </c>
-      <c r="E31">
-        <f>D31-D30</f>
-        <v>1</v>
-      </c>
-      <c r="F31" s="2">
-        <f t="shared" ref="F31:F33" si="20">(B31/B30)^(1/E31)-1</f>
+        <f>C31-C30</f>
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
+        <f>(B31/B30)^(1/D31)-1</f>
         <v>0.17006802721088432</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>43916</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="4">
         <v>858</v>
       </c>
       <c r="C32">
-        <v>38550</v>
+        <f>A32-$A$2</f>
+        <v>61</v>
       </c>
       <c r="D32">
-        <f t="shared" si="19"/>
-        <v>61</v>
-      </c>
-      <c r="E32">
-        <f t="shared" ref="E32:E33" si="21">D32-D31</f>
-        <v>1</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="D32:D33" si="7">C32-C31</f>
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <f>(B32/B31)^(1/D32)-1</f>
         <v>0.24709302325581395</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>43917</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="4">
         <v>993</v>
       </c>
       <c r="C33">
-        <v>41032</v>
+        <f>A33-$A$2</f>
+        <v>62</v>
       </c>
       <c r="D33">
-        <f t="shared" si="19"/>
-        <v>62</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
-      <c r="F33" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E33" s="2">
+        <f>(B33/B32)^(1/D33)-1</f>
         <v>0.15734265734265729</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="F33" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>43918</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1144</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:C42" si="8">A34-$A$2</f>
+        <v>63</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ref="D34:D42" si="9">C34-C33</f>
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" ref="E34:E42" si="10">(B34/B33)^(1/D34)-1</f>
+        <v>0.15206445115810685</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1355</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="10"/>
+        <v>0.18444055944055937</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1706</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="10"/>
+        <v>0.2590405904059041</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1966</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="8"/>
+        <v>66</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="10"/>
+        <v>0.15240328253223923</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B38" s="4">
+        <v>2392</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="8"/>
+        <v>67</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="10"/>
+        <v>0.21668362156663279</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B39" s="4">
+        <v>2793</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="8"/>
+        <v>68</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="10"/>
+        <v>0.16764214046822734</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B40" s="4">
+        <v>3255</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="10"/>
+        <v>0.16541353383458657</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B41" s="4">
+        <v>3630</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="10"/>
+        <v>0.11520737327188946</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B42" s="4">
+        <v>4038</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="8"/>
+        <v>71</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="10"/>
+        <v>0.11239669421487597</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1"/>
-    <hyperlink ref="G9" r:id="rId2"/>
-    <hyperlink ref="G10" r:id="rId3"/>
-    <hyperlink ref="G11" r:id="rId4"/>
-    <hyperlink ref="G12" r:id="rId5"/>
-    <hyperlink ref="G13" r:id="rId6"/>
-    <hyperlink ref="G14" r:id="rId7"/>
-    <hyperlink ref="G15" r:id="rId8"/>
-    <hyperlink ref="G16" r:id="rId9"/>
-    <hyperlink ref="G17" r:id="rId10"/>
-    <hyperlink ref="G18" r:id="rId11"/>
-    <hyperlink ref="G3" r:id="rId12"/>
-    <hyperlink ref="G4" r:id="rId13"/>
-    <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G6" r:id="rId15"/>
-    <hyperlink ref="G7" r:id="rId16"/>
-    <hyperlink ref="G8" r:id="rId17"/>
-    <hyperlink ref="G2" r:id="rId18"/>
-    <hyperlink ref="G20" r:id="rId19"/>
-    <hyperlink ref="G21" r:id="rId20"/>
-    <hyperlink ref="G22" r:id="rId21"/>
-    <hyperlink ref="G23" r:id="rId22"/>
-    <hyperlink ref="G24" r:id="rId23"/>
-    <hyperlink ref="G25" r:id="rId24"/>
-    <hyperlink ref="G26" r:id="rId25"/>
-    <hyperlink ref="G27" r:id="rId26"/>
-    <hyperlink ref="G28" r:id="rId27"/>
-    <hyperlink ref="G29" r:id="rId28"/>
-    <hyperlink ref="G30" r:id="rId29"/>
-    <hyperlink ref="G32" r:id="rId30"/>
-    <hyperlink ref="G31" r:id="rId31"/>
-    <hyperlink ref="G33" r:id="rId32"/>
+    <hyperlink ref="F19" r:id="rId1"/>
+    <hyperlink ref="F9" r:id="rId2"/>
+    <hyperlink ref="F10" r:id="rId3"/>
+    <hyperlink ref="F11" r:id="rId4"/>
+    <hyperlink ref="F12" r:id="rId5"/>
+    <hyperlink ref="F13" r:id="rId6"/>
+    <hyperlink ref="F14" r:id="rId7"/>
+    <hyperlink ref="F15" r:id="rId8"/>
+    <hyperlink ref="F16" r:id="rId9"/>
+    <hyperlink ref="F17" r:id="rId10"/>
+    <hyperlink ref="F18" r:id="rId11"/>
+    <hyperlink ref="F3" r:id="rId12"/>
+    <hyperlink ref="F4" r:id="rId13"/>
+    <hyperlink ref="F5" r:id="rId14"/>
+    <hyperlink ref="F6" r:id="rId15"/>
+    <hyperlink ref="F7" r:id="rId16"/>
+    <hyperlink ref="F8" r:id="rId17"/>
+    <hyperlink ref="F2" r:id="rId18"/>
+    <hyperlink ref="F20" r:id="rId19"/>
+    <hyperlink ref="F21" r:id="rId20"/>
+    <hyperlink ref="F22" r:id="rId21"/>
+    <hyperlink ref="F23" r:id="rId22"/>
+    <hyperlink ref="F24" r:id="rId23"/>
+    <hyperlink ref="F25" r:id="rId24"/>
+    <hyperlink ref="F26" r:id="rId25"/>
+    <hyperlink ref="F27" r:id="rId26"/>
+    <hyperlink ref="F28" r:id="rId27"/>
+    <hyperlink ref="F29" r:id="rId28"/>
+    <hyperlink ref="F30" r:id="rId29"/>
+    <hyperlink ref="F32" r:id="rId30"/>
+    <hyperlink ref="F31" r:id="rId31"/>
+    <hyperlink ref="F33" r:id="rId32"/>
+    <hyperlink ref="F42" r:id="rId33"/>
+    <hyperlink ref="F41" r:id="rId34"/>
+    <hyperlink ref="F39" r:id="rId35"/>
+    <hyperlink ref="F40" r:id="rId36"/>
+    <hyperlink ref="F37" r:id="rId37"/>
+    <hyperlink ref="F38" r:id="rId38"/>
+    <hyperlink ref="F35" r:id="rId39"/>
+    <hyperlink ref="F34" r:id="rId40"/>
+    <hyperlink ref="F36" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId33"/>
+  <drawing r:id="rId42"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>